<commit_message>
added switch add new subscription recurly
</commit_message>
<xml_diff>
--- a/Data/My Administration/Subscription Management.xlsx
+++ b/Data/My Administration/Subscription Management.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\commerce-automation\Data\My Administration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4BE917-FC32-4DEE-A945-3EA3E04CE3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11740" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Subscription Recurly" sheetId="1" r:id="rId1"/>
@@ -120,14 +126,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,346 +142,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -489,253 +159,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -748,62 +176,92 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -819,11 +277,51 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1081,22 +579,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.2890625" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1730,27 +1228,25 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A$1:A$1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.2890625" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1767,7 +1263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="14.8" spans="1:4">
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="5">
         <v>1927334</v>
       </c>
@@ -1993,27 +1489,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A4">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="49.859375" customWidth="1"/>
-    <col min="3" max="3" width="12.4296875" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2062,21 +1554,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
   </cols>
@@ -2098,26 +1588,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="4" max="4" width="28.765625" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2190,7 +1678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" customFormat="1" spans="1:4">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>274113</v>
       </c>
@@ -2204,7 +1692,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="1" spans="1:4">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>279007</v>
       </c>
@@ -2218,7 +1706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" customFormat="1" spans="1:4">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>331968</v>
       </c>
@@ -2232,7 +1720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" customFormat="1" spans="1:4">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>314592</v>
       </c>
@@ -2752,29 +2240,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12:A13">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:A35">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:A41 A43:A45">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:A27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
   </cols>
@@ -2914,11 +2400,21 @@
         <v>1940135</v>
       </c>
     </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="2"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A27">
+    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28">
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit update select DB
</commit_message>
<xml_diff>
--- a/Data/My Administration/Subscription Management.xlsx
+++ b/Data/My Administration/Subscription Management.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\commerce-automation\Data\My Administration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA8D2DF-221C-4AB0-81CA-C11368B180F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="16860" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Subscription Recurly" sheetId="1" r:id="rId1"/>
@@ -102,12 +108,6 @@
     <t>planId</t>
   </si>
   <si>
-    <t>testops_platform_annual, kse_per-user_annual, visual_testing_pro_annual</t>
-  </si>
-  <si>
-    <t>3500, 2, 20000</t>
-  </si>
-  <si>
     <t>kse_per-user_annual, kre_floating_annual</t>
   </si>
   <si>
@@ -115,19 +115,19 @@
   </si>
   <si>
     <t>8</t>
+  </si>
+  <si>
+    <t>testops_platform_annual, visual_testing_pro_annual</t>
+  </si>
+  <si>
+    <t>3500, 20000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,346 +135,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -482,253 +152,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -736,62 +164,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="31">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -820,10 +224,231 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -832,6 +457,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1089,22 +717,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.2890625" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1738,27 +1366,25 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A$1:A$1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="30" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.2890625" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2113,46 +1739,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A5">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A7">
-    <cfRule type="duplicateValues" dxfId="1" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A9">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A25">
-    <cfRule type="duplicateValues" dxfId="1" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="12"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="49.859375" customWidth="1"/>
-    <col min="3" max="3" width="12.4296875" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2171,10 +1795,10 @@
         <v>1940294</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2182,10 +1806,10 @@
         <v>1940297</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2196,30 +1820,28 @@
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A4">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
   </cols>
@@ -2241,23 +1863,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
   </cols>
@@ -2499,40 +2117,38 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="duplicateValues" dxfId="1" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A11 A13:A47 A49:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A11 A13:A19 A21:A29">
-    <cfRule type="duplicateValues" dxfId="1" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="12"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" customWidth="1"/>
@@ -3170,15 +2786,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12:A13">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:A35">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:A41 A43:A45">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>